<commit_message>
renaming apex office print to cloud office print
</commit_message>
<xml_diff>
--- a/examples/spacex_example/output.xlsx
+++ b/examples/spacex_example/output.xlsx
@@ -1647,7 +1647,7 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6191250" cy="2857500"/>
+    <xdr:ext cx="7620000" cy="2857500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2"/>
@@ -2380,7 +2380,7 @@
         <v>90</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="H10" s="0" t="s">
         <v>20</v>

</xml_diff>